<commit_message>
Vectorized Probs function to gain speed.
Added a healthcare use outcome.

Model now saves data snapshots at each time cycle and returns them all in a list object when the run is complete.

Model now prints progress on the console and saves log files for each run.
</commit_message>
<xml_diff>
--- a/Data/parameters wildfire-asthma.xlsx
+++ b/Data/parameters wildfire-asthma.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaya\Box\AA_Sigal_Documents\Climate - Health\Modeling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664E81FA-84CB-4665-9450-2A7815AC5B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8164D681-6896-4FD7-96A5-EFFC480D0E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" xr2:uid="{7E6B6D9A-B1C0-459E-B09F-F2944DC9D3C6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{7E6B6D9A-B1C0-459E-B09F-F2944DC9D3C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Interventions" sheetId="2" r:id="rId2"/>
-    <sheet name="3-state model parameters" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>Parameter</t>
   </si>
@@ -314,185 +313,6 @@
   <si>
     <t>Mean 0.23 visits per person-year. Beta for controlled asthma is -0.153.
 The best predictor of future ed visit and hospitalizations are previous ed visits and hospitalizations (https://pubmed.ncbi.nlm.nih.gov/26667853/)</t>
-  </si>
-  <si>
-    <t>Controlled</t>
-  </si>
-  <si>
-    <t>Partly controlled</t>
-  </si>
-  <si>
-    <t>Uncontrolled</t>
-  </si>
-  <si>
-    <t>0.13-0.16</t>
-  </si>
-  <si>
-    <t>0.73-0.75</t>
-  </si>
-  <si>
-    <t>0.064-0.10</t>
-  </si>
-  <si>
-    <t>0.19-0.21</t>
-  </si>
-  <si>
-    <t>0.057-0.061</t>
-  </si>
-  <si>
-    <t>0.71-0.74</t>
-  </si>
-  <si>
-    <t>0.18-0.19</t>
-  </si>
-  <si>
-    <t>0.012-0.023</t>
-  </si>
-  <si>
-    <t>0.81-0.85</t>
-  </si>
-  <si>
-    <t>Prob exacerbation if controlled</t>
-  </si>
-  <si>
-    <t>0.08 - 0.18 %</t>
-  </si>
-  <si>
-    <t>Prob exacerbation if partly controlled</t>
-  </si>
-  <si>
-    <t>Prob exacerbation if uncontrolled</t>
-  </si>
-  <si>
-    <t>0.49 - 1.1 %</t>
-  </si>
-  <si>
-    <t>0.20 - 0.35 %</t>
-  </si>
-  <si>
-    <t>Bateman 2010 (Table II)</t>
-  </si>
-  <si>
-    <t>Probs for 1 week</t>
-  </si>
-  <si>
-    <t>To:</t>
-  </si>
-  <si>
-    <t>From:</t>
-  </si>
-  <si>
-    <t>Note that this is transposed from the original table in the paper</t>
-  </si>
-  <si>
-    <t>The ranges reflect different medications</t>
-  </si>
-  <si>
-    <t>OR for an exacerbation in subsequent weeks was 1.97 for partly controlled vs controlled week. 
-2.91 for uncontrolled vs. partly controlled week. 
-5.74 for uncontrolled. Vs controlled week.</t>
-  </si>
-  <si>
-    <t>Empirical data from multiple clinical studies</t>
-  </si>
-  <si>
-    <t>Controlled = all 5 subcriteria were controlled and no severe exacerbations</t>
-  </si>
-  <si>
-    <t>Partly controlled = 1-2 subcriteria were uncontrolled and no severe exacerbation</t>
-  </si>
-  <si>
-    <t>Uncontrolled = 3+ subcriteria uncontrolled or had an exacerbation</t>
-  </si>
-  <si>
-    <t>Totally controlled</t>
-  </si>
-  <si>
-    <t>Well-controlled</t>
-  </si>
-  <si>
-    <t>Not well controlled (no exacerbation)</t>
-  </si>
-  <si>
-    <t>Not well controlled (with exacerbation)</t>
-  </si>
-  <si>
-    <t>0.837 - 0.894</t>
-  </si>
-  <si>
-    <t>0.078 - 0.122</t>
-  </si>
-  <si>
-    <t>0.028 - 0.039</t>
-  </si>
-  <si>
-    <t>0.001 - 0.002</t>
-  </si>
-  <si>
-    <t>0.121 - 0.188</t>
-  </si>
-  <si>
-    <t>0.109 - 0.141</t>
-  </si>
-  <si>
-    <t>0.001 - 0.004</t>
-  </si>
-  <si>
-    <t>0.028 - 0.070</t>
-  </si>
-  <si>
-    <t>0.122 - 0.171</t>
-  </si>
-  <si>
-    <t>0.755 - 0.844</t>
-  </si>
-  <si>
-    <t>0.003 - 0.006</t>
-  </si>
-  <si>
-    <t>0.046 - 0.152</t>
-  </si>
-  <si>
-    <t>0.094 - 0.215</t>
-  </si>
-  <si>
-    <t>0.141 - 0.213</t>
-  </si>
-  <si>
-    <t>0.569 - 0.637</t>
-  </si>
-  <si>
-    <t>Empirical data from the "maintenance" phase of a clinical trial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Study began with a "dose escalation" phase where tx was stepped up every 12 weeks until asthma was totally controlled or max dose was reached. Patients who achieve total control or complete 12 weeks (whichever came first) entered the "maintencance" phase, and remained on the same dose until the end of the study. </t>
-  </si>
-  <si>
-    <t>Bateman 2008 (Table 1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exacerbation = "deterioration in asthma resulting in hospitalization/ED treatment and/or oral steroid use." It is used as an acute event with no defined duration. </t>
-  </si>
-  <si>
-    <t>Exacerbations defined as part of health states</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The ranges in the table reflect different levels of ICS use at initiation (which reflects baseline control) </t>
-  </si>
-  <si>
-    <t>0.700 - 0.734</t>
-  </si>
-  <si>
-    <t>totally controlled = "none of the following each week: daytime symptoms, use of rescue salbutamol/albuterol, night-time awakenings, exacerbations (defined as a deterioration in asthma requiring treatment with an oral corticosteroid or an emergency department visit, and/or hospitalization), emergency visits or treatment-related adverse events (AE) enforcing a change in therapy. In addition, patients had a morning PEF of ≥ 80% predicted for every day."</t>
-  </si>
-  <si>
-    <t>well-controlled = "same criteria as total control for night-time awakenings, exacerbations, emergency visits, and treatment-related AE. Patients also had to achieve two out of the following: ≤2 days with a daytime symptom score &gt;1; ≤2 days and ≤4 occasions of rescue medication use; or morning PEF ≥80% predicted every day."</t>
-  </si>
-  <si>
-    <t>This group would include both "well controlled" and "partly controlled" people per GINA</t>
-  </si>
-  <si>
-    <t>This group would be considered "well controlled" per GINA</t>
   </si>
 </sst>
 </file>
@@ -503,7 +323,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,15 +355,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -571,7 +382,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -748,27 +559,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -876,17 +672,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -943,18 +730,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1274,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184F7F09-0BD7-4EAE-BD5B-051F2BA75746}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1301,20 +1076,20 @@
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="42"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="13" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="42"/>
+      <c r="G1" s="39"/>
       <c r="H1" s="13" t="s">
         <v>10</v>
       </c>
@@ -1361,85 +1136,85 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="40" t="s">
         <v>57</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>61</v>
       </c>
       <c r="C4" s="21"/>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="55" t="s">
+      <c r="E4" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="51">
+      <c r="G4" s="48">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="I4" s="55" t="s">
+      <c r="I4" s="52" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="44"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="56"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="53"/>
     </row>
     <row r="6" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="44"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="56"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="53"/>
     </row>
     <row r="7" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="44"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C7" s="26">
         <v>0.251</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="56"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="53"/>
     </row>
     <row r="8" spans="1:11" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="45"/>
+      <c r="A8" s="42"/>
       <c r="B8" s="19" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="27">
         <v>0.29299999999999998</v>
       </c>
-      <c r="D8" s="54"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="57"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="54"/>
     </row>
     <row r="9" spans="1:11" ht="261.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
@@ -1464,7 +1239,7 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="40" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="17" t="s">
@@ -1479,57 +1254,57 @@
       <c r="E10" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="58" t="s">
+      <c r="I10" s="55" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="44"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="17" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="F11" s="49"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-      <c r="I11" s="59"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="56"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="44"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="17" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-      <c r="I12" s="56"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="53"/>
     </row>
     <row r="13" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="10"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="56"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="53"/>
     </row>
     <row r="14" spans="1:11" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="45"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="17" t="s">
         <v>49</v>
       </c>
@@ -1543,13 +1318,13 @@
       <c r="E14" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="57"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="54"/>
     </row>
     <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="40" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="21" t="s">
@@ -1564,20 +1339,20 @@
       <c r="I15" s="23"/>
     </row>
     <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="20" t="s">
         <v>27</v>
       </c>
       <c r="E16" s="20"/>
     </row>
     <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="45"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
@@ -1590,7 +1365,7 @@
       <c r="I18" s="25"/>
     </row>
     <row r="19" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="40" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="18" t="s">
@@ -1612,19 +1387,19 @@
       <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="44"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="44"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="45"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="19" t="s">
         <v>32</v>
       </c>
@@ -1637,7 +1412,7 @@
       <c r="I22" s="25"/>
     </row>
     <row r="23" spans="1:9" ht="87" x14ac:dyDescent="0.35">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="40" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="18" t="s">
@@ -1659,19 +1434,19 @@
       <c r="I23" s="23"/>
     </row>
     <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="44"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="44"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="45"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="19" t="s">
         <v>37</v>
       </c>
@@ -1684,7 +1459,7 @@
       <c r="I26" s="25"/>
     </row>
     <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="43" t="s">
+      <c r="A27" s="40" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="18" t="s">
@@ -1706,19 +1481,19 @@
       <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="44"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="17" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="44"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="17" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="45"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="19" t="s">
         <v>40</v>
       </c>
@@ -1731,7 +1506,7 @@
       <c r="I30" s="25"/>
     </row>
     <row r="31" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="40" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="18" t="s">
@@ -1753,20 +1528,20 @@
       <c r="I31" s="23"/>
     </row>
     <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A32" s="44"/>
+      <c r="A32" s="41"/>
       <c r="B32" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A33" s="44"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="17" t="s">
         <v>44</v>
       </c>
       <c r="I33" s="34"/>
     </row>
     <row r="34" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="45"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="19" t="s">
         <v>45</v>
       </c>
@@ -1785,7 +1560,7 @@
       <c r="I35" s="34"/>
     </row>
     <row r="36" spans="1:9" ht="145" x14ac:dyDescent="0.35">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="40" t="s">
         <v>66</v>
       </c>
       <c r="B36" s="18" t="s">
@@ -1812,7 +1587,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="45"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="19"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24" t="s">
@@ -1828,7 +1603,7 @@
       <c r="H37" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="I37" s="63" t="s">
+      <c r="I37" s="37" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1880,7 +1655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E9FB14E-8BB6-4734-A031-4EAA67385DF3}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -1902,319 +1677,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D859F13B-7793-4FCD-9443-B460C97F381D}">
-  <dimension ref="A1:K19"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.7265625" style="37"/>
-    <col min="2" max="2" width="20.1796875" style="37" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="12" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="13.08984375" style="37" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="37"/>
-    <col min="10" max="10" width="66.1796875" style="37" customWidth="1"/>
-    <col min="11" max="11" width="21" style="37" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="37"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-    </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="61"/>
-      <c r="B3" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="61"/>
-      <c r="B4" s="37" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="61"/>
-      <c r="B5" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="F5" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="61"/>
-    </row>
-    <row r="7" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="61"/>
-      <c r="B7" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A8" s="61"/>
-      <c r="B8" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>102</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="61"/>
-      <c r="B9" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="61"/>
-    </row>
-    <row r="11" spans="1:11" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="61"/>
-      <c r="B11" s="37" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="61" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="38"/>
-    </row>
-    <row r="15" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="61"/>
-      <c r="B15" s="37" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="G15" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="H15" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="J15" s="37" t="s">
-        <v>143</v>
-      </c>
-      <c r="K15" s="37" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="98.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="61"/>
-      <c r="B16" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C16" s="60" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="F16" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="G16" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="H16" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="J16" s="37" t="s">
-        <v>144</v>
-      </c>
-      <c r="K16" s="37" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="61"/>
-      <c r="B17" s="37" t="s">
-        <v>141</v>
-      </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="G17" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="H17" s="38" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="61"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="F18" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="G18" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="H18" s="38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="61"/>
-      <c r="B19" s="37" t="s">
-        <v>140</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="F19" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="G19" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H19" s="38" t="s">
-        <v>135</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="A14:A19"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A2:A11"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A2:A11" r:id="rId1" display="Bateman 2010 (Table II)" xr:uid="{7A69B00F-FD9D-4359-B8A7-233D67495178}"/>
-    <hyperlink ref="A14:A19" r:id="rId2" display="Bateman 2008 (Table 1)" xr:uid="{32EB0C55-03CB-4B94-9D72-3E5FD93B7C46}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
-</worksheet>
 </file>
</xml_diff>